<commit_message>
making columns right in pandas
</commit_message>
<xml_diff>
--- a/all_courses.xlsx
+++ b/all_courses.xlsx
@@ -55,10 +55,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -427,7 +430,7 @@
   </sheetPr>
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -481,45 +484,45 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
+      <c r="A2" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" s="2" t="inlineStr">
         <is>
           <t>خیاطی</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" s="2" t="inlineStr">
         <is>
           <t>مهدیه کوله باری</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="D2" s="2" t="inlineStr">
         <is>
           <t>55</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="E2" s="2" t="inlineStr">
         <is>
           <t>1402/11/30</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="F2" s="2" t="inlineStr">
         <is>
           <t>1402/12/24</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="G2" s="2" t="inlineStr">
         <is>
           <t>مشهد</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="H2" s="2" t="inlineStr">
         <is>
           <t>فنی حرفه ای ۱۴</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="I2" s="2" t="inlineStr">
         <is>
           <t>زن</t>
         </is>

</xml_diff>